<commit_message>
Fix precinct names to match sample CSV
This update will completely process the sample CSV, including fixed
typos on precinct names, added a shape for Chamblee 2, and will ignore
Marietta 5B (too small a precinct to rely on having results)
</commit_message>
<xml_diff>
--- a/GA06_block_map.xlsx
+++ b/GA06_block_map.xlsx
@@ -12102,7 +12102,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>CHAMBLEE</t>
+          <t>CHAMBLEE 2</t>
         </r>
       </text>
     </comment>
@@ -12116,7 +12116,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>CHAMBLEE</t>
+          <t>CHAMBLEE 2</t>
         </r>
       </text>
     </comment>
@@ -12354,7 +12354,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>CHAMBLEE</t>
+          <t>CHAMBLEE 2</t>
         </r>
       </text>
     </comment>
@@ -12368,7 +12368,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>CHAMBLEE</t>
+          <t>CHAMBLEE 2</t>
         </r>
       </text>
     </comment>
@@ -12382,7 +12382,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>CHAMBLEE</t>
+          <t>CHAMBLEE 2</t>
         </r>
       </text>
     </comment>
@@ -14029,7 +14029,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="208">
   <si>
     <t>ML021</t>
   </si>
@@ -14650,6 +14650,9 @@
   </si>
   <si>
     <t>BRIARLAKE ELEM</t>
+  </si>
+  <si>
+    <t>CHAMBLEE 2</t>
   </si>
 </sst>
 </file>
@@ -16446,8 +16449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AR32" sqref="AR32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19108,11 +19111,11 @@
       <c r="AB34" s="176" t="s">
         <v>175</v>
       </c>
-      <c r="AC34" s="183" t="s">
-        <v>182</v>
-      </c>
-      <c r="AD34" s="183" t="s">
-        <v>182</v>
+      <c r="AC34" s="136" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD34" s="136" t="s">
+        <v>207</v>
       </c>
       <c r="AE34" s="184" t="s">
         <v>183</v>
@@ -19164,14 +19167,14 @@
       <c r="AA35" s="187" t="s">
         <v>186</v>
       </c>
-      <c r="AB35" s="183" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC35" s="183" t="s">
-        <v>182</v>
-      </c>
-      <c r="AD35" s="183" t="s">
-        <v>182</v>
+      <c r="AB35" s="136" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC35" s="136" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD35" s="136" t="s">
+        <v>207</v>
       </c>
       <c r="AE35" s="183" t="s">
         <v>182</v>

</xml_diff>